<commit_message>
Add 4 missing countries
</commit_message>
<xml_diff>
--- a/REE_countries.xlsx
+++ b/REE_countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HopesAndDreams\Dropbox (uwamath)\PUBPOL_GovAnalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0EC5A9-996A-478B-AAD6-B43445F7A8FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25CDB24-B25C-4C7C-AA78-B1C26545E119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8620" yWindow="4130" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="196">
   <si>
     <t>Cuba</t>
   </si>
@@ -601,9 +601,6 @@
     <t>North Korea</t>
   </si>
   <si>
-    <t>Palestinian territories</t>
-  </si>
-  <si>
     <t>Sahrawi Arab Democratic Republic</t>
   </si>
   <si>
@@ -611,6 +608,18 @@
   </si>
   <si>
     <t>Developing</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Palestine</t>
   </si>
 </sst>
 </file>
@@ -986,20 +995,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B143"/>
+  <dimension ref="A1:B147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" t="s">
         <v>191</v>
-      </c>
-      <c r="B1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2280,8 +2289,44 @@
         <v>1</v>
       </c>
     </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>192</v>
+      </c>
+      <c r="B144">
+        <f>IF(COUNTIF(other!$A$1:$A$158,A144),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>193</v>
+      </c>
+      <c r="B145">
+        <f>IF(COUNTIF(other!$A$1:$A$158,A145),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>194</v>
+      </c>
+      <c r="B146">
+        <f>IF(COUNTIF(other!$A$1:$A$158,A146),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>195</v>
+      </c>
+      <c r="B147">
+        <f>IF(COUNTIF(other!$A$1:$A$158,A147),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:A143">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A143">
     <sortCondition ref="A2:A143"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2292,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A20F91-086E-4266-BE87-952FA7761FE5}">
   <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2315,7 +2360,7 @@
         <v>59</v>
       </c>
       <c r="B2">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A2),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A2),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2324,7 +2369,7 @@
         <v>42</v>
       </c>
       <c r="B3">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A3),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A3),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2333,7 +2378,7 @@
         <v>53</v>
       </c>
       <c r="B4">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A4),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A4),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2342,7 +2387,7 @@
         <v>142</v>
       </c>
       <c r="B5">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A5),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A5),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2351,7 +2396,7 @@
         <v>99</v>
       </c>
       <c r="B6">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A6),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A6),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2360,7 +2405,7 @@
         <v>80</v>
       </c>
       <c r="B7">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A7),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A7),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2369,7 +2414,7 @@
         <v>143</v>
       </c>
       <c r="B8">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A8),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A8),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2378,7 +2423,7 @@
         <v>77</v>
       </c>
       <c r="B9">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A9),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A9),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2387,7 +2432,7 @@
         <v>144</v>
       </c>
       <c r="B10">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A10),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A10),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2396,7 +2441,7 @@
         <v>111</v>
       </c>
       <c r="B11">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A11),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A11),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2405,7 +2450,7 @@
         <v>137</v>
       </c>
       <c r="B12">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A12),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A12),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2414,7 +2459,7 @@
         <v>145</v>
       </c>
       <c r="B13">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A13),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A13),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2423,7 +2468,7 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A14),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A14),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2432,7 +2477,7 @@
         <v>50</v>
       </c>
       <c r="B15">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A15),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A15),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2441,7 +2486,7 @@
         <v>108</v>
       </c>
       <c r="B16">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A16),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A16),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2450,7 +2495,7 @@
         <v>146</v>
       </c>
       <c r="B17">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A17),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A17),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2459,7 +2504,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A18),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A18),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2468,7 +2513,7 @@
         <v>15</v>
       </c>
       <c r="B19">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A19),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A19),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2477,7 +2522,7 @@
         <v>48</v>
       </c>
       <c r="B20">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A20),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A20),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2486,7 +2531,7 @@
         <v>34</v>
       </c>
       <c r="B21">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A21),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A21),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2495,7 +2540,7 @@
         <v>147</v>
       </c>
       <c r="B22">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A22),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A22),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2504,7 +2549,7 @@
         <v>35</v>
       </c>
       <c r="B23">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A23),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A23),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2513,7 +2558,7 @@
         <v>89</v>
       </c>
       <c r="B24">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A24),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A24),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2522,7 +2567,7 @@
         <v>116</v>
       </c>
       <c r="B25">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A25),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A25),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2531,7 +2576,7 @@
         <v>103</v>
       </c>
       <c r="B26">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A26),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A26),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2540,7 +2585,7 @@
         <v>120</v>
       </c>
       <c r="B27">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A27),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A27),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2549,7 +2594,7 @@
         <v>148</v>
       </c>
       <c r="B28">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A28),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A28),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2558,7 +2603,7 @@
         <v>125</v>
       </c>
       <c r="B29">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A29),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A29),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2567,26 +2612,26 @@
         <v>132</v>
       </c>
       <c r="B30">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A30),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A30),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="B31">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A31),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A31),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
       <c r="B32">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A32),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A32),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -2594,7 +2639,7 @@
         <v>65</v>
       </c>
       <c r="B33">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A33),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A33),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2603,503 +2648,503 @@
         <v>70</v>
       </c>
       <c r="B34">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A34),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A34),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B35">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A35),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A35),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="B36">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A36),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A36),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="B37">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A37),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A37),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="B38">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A38),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A38),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>192</v>
       </c>
       <c r="B39">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A39),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A39),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
       <c r="B40">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A40),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A40),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A41),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A41),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="B42">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A42),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A42),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="B43">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A43),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A43),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A44),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A44),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B45">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A45),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A45),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
       <c r="B46">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A46),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A46),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B47">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A47),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A47),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A48),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A48),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="B49">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A49),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A49),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="B50">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A50),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A50),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="B51">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A51),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A51),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B52">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A52),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A52),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
       <c r="B53">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A53),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A53),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="B54">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A54),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A54),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>92</v>
       </c>
       <c r="B55">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A55),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A55),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B56">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A56),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A56),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="B57">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A57),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A57),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="B58">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A58),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A58),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B59">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A59),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A59),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="B60">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A60),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A60),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B61">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A61),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A61),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="B62">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A62),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A62),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
       <c r="B63">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A63),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A63),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B64">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A64),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A64),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="B65">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A65),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A65),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="B66">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A66),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A66),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B67">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A67),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A67),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B68">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A68),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A68),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B69">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A69),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A69),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B70">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A70),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A70),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="B71">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A71),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A71),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B72">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A72),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A72),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>161</v>
       </c>
       <c r="B73">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A73),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A73),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B74">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A74),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A74),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="B75">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A75),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A75),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B76">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A76),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A76),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="B77">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A77),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A77),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="B78">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A78),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A78),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
       <c r="B79">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A79),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A79),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="B80">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A80),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A80),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B81">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A81),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A81),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B82">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A82),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A82),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="B83">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A83),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A83),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>164</v>
       </c>
       <c r="B84">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A84),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A84),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>96</v>
       </c>
       <c r="B85">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A85),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A85),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="B86">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A86),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A86),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>60</v>
       </c>
       <c r="B87">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A87),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A87),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="B88">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A88),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A88),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="B89">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A89),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A89),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -3107,7 +3152,7 @@
         <v>49</v>
       </c>
       <c r="B90">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A90),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A90),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3116,7 +3161,7 @@
         <v>168</v>
       </c>
       <c r="B91">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A91),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A91),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3125,7 +3170,7 @@
         <v>32</v>
       </c>
       <c r="B92">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A92),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A92),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3134,7 +3179,7 @@
         <v>90</v>
       </c>
       <c r="B93">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A93),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A93),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3143,7 +3188,7 @@
         <v>62</v>
       </c>
       <c r="B94">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A94),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A94),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3152,7 +3197,7 @@
         <v>131</v>
       </c>
       <c r="B95">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A95),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A95),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3161,7 +3206,7 @@
         <v>43</v>
       </c>
       <c r="B96">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A96),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A96),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3170,7 +3215,7 @@
         <v>169</v>
       </c>
       <c r="B97">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A97),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A97),1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3179,7 +3224,7 @@
         <v>74</v>
       </c>
       <c r="B98">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A98),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A98),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3188,7 +3233,7 @@
         <v>58</v>
       </c>
       <c r="B99">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A99),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A99),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3197,7 +3242,7 @@
         <v>87</v>
       </c>
       <c r="B100">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A100),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A100),1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3206,525 +3251,528 @@
         <v>141</v>
       </c>
       <c r="B101">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A101),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A101),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="B102">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A102),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A102),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="B103">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A103),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A103),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="B104">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A104),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A104),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="B105">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A105),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A105),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
       <c r="B106">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A106),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A106),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="B107">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A107),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A107),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="B108">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A108),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A108),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
       <c r="B109">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A109),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A109),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B110">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A110),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A110),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B111">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A111),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A111),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="B112">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A112),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A112),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B113">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A113),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A113),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="B114">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A114),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A114),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B115">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A115),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A115),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="B116">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A116),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A116),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="B117">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A117),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A117),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B118">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A118),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A118),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B119">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A119),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A119),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B120">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A120),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A120),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="B121">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A121),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A121),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="B122">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A122),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A122),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="B123">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A123),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A123),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>178</v>
+        <v>68</v>
       </c>
       <c r="B124">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A124),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A124),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>179</v>
+        <v>97</v>
       </c>
       <c r="B125">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A125),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A125),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>180</v>
+        <v>18</v>
       </c>
       <c r="B126">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A126),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A126),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B127">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A127),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A127),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="B128">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A128),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A128),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B129">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A129),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A129),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="B130">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A130),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A130),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="B131">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A131),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A131),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B132">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A132),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A132),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B133">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A133),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A133),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="B134">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A134),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A134),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
       <c r="B135">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A135),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A135),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B136">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A136),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A136),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>184</v>
+        <v>45</v>
       </c>
       <c r="B137">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A137),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A137),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="B138">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A138),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A138),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>185</v>
+        <v>122</v>
       </c>
       <c r="B139">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A139),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A139),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="B140">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A140),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A140),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>72</v>
+        <v>184</v>
       </c>
       <c r="B141">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A141),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A141),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B142">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A142),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A142),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>124</v>
+        <v>185</v>
       </c>
       <c r="B143">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A143),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A143),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="B144">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A144),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A144),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="B145">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A145),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A145),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B146">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A146),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A146),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="B147">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A147),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A147),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>47</v>
+        <v>186</v>
       </c>
       <c r="B148">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A148),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A148),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="B149">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A149),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A149),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B150">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A150),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A150),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B151">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A151),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A151),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>139</v>
+        <v>47</v>
       </c>
       <c r="B152">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A152),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A152),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="B153">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A153),1,0)</f>
-        <v>1</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A153),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="B154">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A154),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A154),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="B155">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A155),1,0)</f>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A155),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="B156">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A156),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A156),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="B157">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A157),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A157),1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
       <c r="B158">
-        <f>IF(COUNTIF(Sheet1!$A$2:$A$143,A158),1,0)</f>
-        <v>0</v>
+        <f>IF(COUNTIF(Sheet1!$A$2:$A$147,A158),1,0)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:B161" xr:uid="{479FEAF1-2229-488A-825D-DFA1CCBEB4F7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B158">
+    <sortCondition ref="A151"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>